<commit_message>
new file:   "Kindle/071/\343\201\225\343\202\211\343\201\260\345\274\201\350\255\267\345\243\253\351\211\204\351\201\223071\357\274\217\346\227\245\346\234\254\345\274\201\350\255\267\345\243\253\351\200\243\345\220\210\344\274\232\343\203\273\345\260\217\346\236\227\345\205\203\346\262\273\344\274\232\351\225\267\343\201\253\345\257\276\343\201\231\343\202\213\346\261\202\346\204\217\350\246\213\346\233\270.pdf" 	modified:   n 	modified:   "\351\200\232\350\251\261\350\250\230\351\214\262.xlsx"
update 2023-11-28_1757 DESKTOP-1ASSOGN
</commit_message>
<xml_diff>
--- a/通話記録.xlsx
+++ b/通話記録.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\a66\git\kk2023_07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BFC842-B3FE-49A2-BAE0-63204CAFF31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0CD62D-07CC-44A0-86D2-5B73356B66D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15690" yWindow="1170" windowWidth="18795" windowHeight="11160" xr2:uid="{29DE34D1-672B-AD4C-953D-8C85BF37DDE2}"/>
+    <workbookView xWindow="12420" yWindow="2115" windowWidth="18795" windowHeight="11160" xr2:uid="{29DE34D1-672B-AD4C-953D-8C85BF37DDE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="71">
   <si>
     <t>金沢弁護士会</t>
     <rPh sb="0" eb="6">
@@ -425,6 +425,41 @@
   </si>
   <si>
     <t>34秒</t>
+    <rPh sb="2" eb="3">
+      <t>ビョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>10分</t>
+    <rPh sb="2" eb="3">
+      <t>フン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>55秒</t>
+    <rPh sb="2" eb="3">
+      <t>ビョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>49秒</t>
+    <rPh sb="2" eb="3">
+      <t>ビョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3分</t>
+    <rPh sb="1" eb="2">
+      <t>フン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>59秒</t>
     <rPh sb="2" eb="3">
       <t>ビョウ</t>
     </rPh>
@@ -802,21 +837,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62500BC-39A4-2D48-9B1D-6CF2F721866A}">
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:J83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5" outlineLevelCol="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.88671875" customWidth="1"/>
-    <col min="10" max="10" width="59.88671875" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="7" width="4.109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="8.5546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="5.88671875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="59.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
@@ -3241,7 +3276,7 @@
         <v>64</v>
       </c>
       <c r="J81" t="str">
-        <f t="shared" ref="J81:J83" si="4">A81 &amp; "・" &amp; B81 &amp; "：" &amp; C81 &amp; "年" &amp; D81 &amp; "月" &amp; E81 &amp; "日" &amp; F81 &amp; "時" &amp;G81 &amp; "分" &amp; "（通話時間" &amp;H81 &amp;"）"</f>
+        <f t="shared" ref="J81:J90" si="4">A81 &amp; "・" &amp; B81 &amp; "：" &amp; C81 &amp; "年" &amp; D81 &amp; "月" &amp; E81 &amp; "日" &amp; F81 &amp; "時" &amp;G81 &amp; "分" &amp; "（通話時間" &amp;H81 &amp;"）"</f>
         <v>国立国会図書館・発信：2023年11月14日13時27分（通話時間9分）</v>
       </c>
     </row>
@@ -3306,24 +3341,253 @@
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
+      <c r="A84" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84">
+        <v>2023</v>
+      </c>
+      <c r="D84" s="1">
+        <v>11</v>
+      </c>
+      <c r="E84" s="1">
+        <v>21</v>
+      </c>
+      <c r="F84" s="1">
+        <v>9</v>
+      </c>
+      <c r="G84" s="1">
+        <v>14</v>
+      </c>
+      <c r="H84" t="s">
+        <v>66</v>
+      </c>
+      <c r="J84" t="str">
+        <f t="shared" si="4"/>
+        <v>金沢弁護士会・発信：2023年11月21日9時14分（通話時間10分）</v>
+      </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
+      <c r="A85" t="s">
+        <v>1</v>
+      </c>
+      <c r="B85" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85">
+        <v>2023</v>
+      </c>
+      <c r="D85" s="1">
+        <v>11</v>
+      </c>
+      <c r="E85" s="1">
+        <v>21</v>
+      </c>
+      <c r="F85" s="1">
+        <v>9</v>
+      </c>
+      <c r="G85" s="1">
+        <v>29</v>
+      </c>
+      <c r="H85" t="s">
+        <v>51</v>
+      </c>
+      <c r="J85" t="str">
+        <f t="shared" si="4"/>
+        <v>金沢地方検察庁・発信：2023年11月21日9時29分（通話時間10分）</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" t="s">
+        <v>4</v>
+      </c>
+      <c r="C86">
+        <v>2023</v>
+      </c>
+      <c r="D86" s="1">
+        <v>11</v>
+      </c>
+      <c r="E86" s="1">
+        <v>21</v>
+      </c>
+      <c r="F86" s="1">
+        <v>15</v>
+      </c>
+      <c r="G86" s="1">
+        <v>1</v>
+      </c>
+      <c r="H86" t="s">
+        <v>67</v>
+      </c>
+      <c r="J86" t="str">
+        <f t="shared" si="4"/>
+        <v>金沢弁護士会・発信：2023年11月21日15時1分（通話時間55秒）</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A87" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87">
+        <v>2023</v>
+      </c>
+      <c r="D87" s="1">
+        <v>11</v>
+      </c>
+      <c r="E87" s="1">
+        <v>21</v>
+      </c>
+      <c r="F87" s="1">
+        <v>15</v>
+      </c>
+      <c r="G87" s="1">
+        <v>15</v>
+      </c>
+      <c r="H87" t="s">
+        <v>68</v>
+      </c>
+      <c r="J87" t="str">
+        <f t="shared" si="4"/>
+        <v>金沢地方裁判所刑事部・発信：2023年11月21日15時15分（通話時間49秒）</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A88" t="s">
+        <v>2</v>
+      </c>
+      <c r="B88" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88">
+        <v>2023</v>
+      </c>
+      <c r="D88" s="1">
+        <v>11</v>
+      </c>
+      <c r="E88" s="1">
+        <v>21</v>
+      </c>
+      <c r="F88" s="1">
+        <v>15</v>
+      </c>
+      <c r="G88" s="1">
+        <v>37</v>
+      </c>
+      <c r="H88" t="s">
+        <v>31</v>
+      </c>
+      <c r="J88" t="str">
+        <f t="shared" si="4"/>
+        <v>金沢地方裁判所刑事部・着信：2023年11月21日15時37分（通話時間12分）</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A89" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89">
+        <v>2023</v>
+      </c>
+      <c r="D89" s="1">
+        <v>11</v>
+      </c>
+      <c r="E89" s="1">
+        <v>21</v>
+      </c>
+      <c r="F89" s="1">
+        <v>15</v>
+      </c>
+      <c r="G89" s="1">
+        <v>59</v>
+      </c>
+      <c r="H89" t="s">
+        <v>69</v>
+      </c>
+      <c r="J89" t="str">
+        <f t="shared" si="4"/>
+        <v>金沢弁護士会・発信：2023年11月21日15時59分（通話時間3分）</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A90" t="s">
+        <v>1</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90">
+        <v>2023</v>
+      </c>
+      <c r="D90" s="1">
+        <v>11</v>
+      </c>
+      <c r="E90" s="1">
+        <v>21</v>
+      </c>
+      <c r="F90" s="1">
+        <v>16</v>
+      </c>
+      <c r="G90" s="1">
+        <v>4</v>
+      </c>
+      <c r="H90" t="s">
+        <v>70</v>
+      </c>
+      <c r="J90" t="str">
+        <f t="shared" si="4"/>
+        <v>金沢地方検察庁・発信：2023年11月21日16時4分（通話時間59秒）</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A91" t="s">
+        <v>1</v>
+      </c>
+      <c r="B91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91">
+        <v>2023</v>
+      </c>
+      <c r="D91" s="1">
+        <v>11</v>
+      </c>
+      <c r="E91" s="1">
+        <v>21</v>
+      </c>
+      <c r="F91" s="1">
+        <v>16</v>
+      </c>
+      <c r="G91" s="1">
+        <v>15</v>
+      </c>
+      <c r="H91" t="s">
+        <v>24</v>
+      </c>
+      <c r="J91" t="str">
+        <f t="shared" ref="J91" si="5">A91 &amp; "・" &amp; B91 &amp; "：" &amp; C91 &amp; "年" &amp; D91 &amp; "月" &amp; E91 &amp; "日" &amp; F91 &amp; "時" &amp;G91 &amp; "分" &amp; "（通話時間" &amp;H91 &amp;"）"</f>
+        <v>金沢地方検察庁・発信：2023年11月21日16時15分（通話時間5分）</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="2">
-    <dataValidation imeMode="halfAlpha" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:G2 C30:D30 C3:D17 D18:D29 C18:C85 D31:D85" xr:uid="{FC87B28D-46EB-794F-B722-AFA6833F59E0}"/>
-    <dataValidation imeMode="on" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{584B5254-0222-5440-B13C-AF680EA701C4}"/>
+    <dataValidation imeMode="halfAlpha" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:G2 C30:D30 C3:D17 D18:D29 D31:D91 C18:C91" xr:uid="{FC87B28D-46EB-794F-B722-AFA6833F59E0}"/>
+    <dataValidation imeMode="on" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{91DF09AD-F9EC-473F-8776-18A42364E802}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
@@ -3333,7 +3597,7 @@
           </x14:formula1>
           <xm:sqref>A2:A20 A25:A37</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BAADC629-B2D9-F94C-9BA8-5308A4393064}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7861D06A-FC34-4343-AA51-CF46E5962B8D}">
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$5</xm:f>
           </x14:formula1>
@@ -3343,7 +3607,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B85</xm:sqref>
+          <xm:sqref>B2:B91</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{968F5D35-0917-F541-BF58-D388F49C2EAA}">
           <x14:formula1>
@@ -3355,7 +3619,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A66:A80 A82:A85</xm:sqref>
+          <xm:sqref>A66:A80 A82:A91</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C9B2EDDF-0896-489E-9C5C-9EDECDF14BB1}">
           <x14:formula1>

</xml_diff>